<commit_message>
More updates to time between injuries analysis
</commit_message>
<xml_diff>
--- a/sims_data_2.xlsx
+++ b/sims_data_2.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C2">
@@ -553,7 +553,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C3">
@@ -641,7 +641,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C4">
@@ -719,7 +719,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C5">
@@ -807,7 +807,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C6">
@@ -895,7 +895,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C7">
@@ -983,7 +983,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C8">
@@ -1071,7 +1071,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C9">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C10">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C12">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C14">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C15">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C16">
@@ -1745,7 +1745,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C17">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C18">
@@ -1911,7 +1911,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C19">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C20">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C21">
@@ -2165,7 +2165,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C22">
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C23">
@@ -2331,7 +2331,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C24">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C27">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C28">
@@ -2844,7 +2844,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C30">
@@ -2932,7 +2932,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C31">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C33">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C35">
@@ -3362,7 +3362,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C36">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C37">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C38">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C39">
@@ -3694,7 +3694,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C40">
@@ -3782,7 +3782,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C41">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C42">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C43">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C44">
@@ -4104,7 +4104,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C45">
@@ -4192,7 +4192,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C46">
@@ -4270,7 +4270,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C47">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C48">
@@ -4426,7 +4426,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C49">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C50">
@@ -4562,7 +4562,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C51">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C52">
@@ -4738,7 +4738,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C53">
@@ -4992,7 +4992,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C56">
@@ -5080,7 +5080,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C57">
@@ -5168,7 +5168,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C58">
@@ -5246,7 +5246,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C59">
@@ -5334,7 +5334,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C60">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C61">
@@ -5510,7 +5510,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C62">
@@ -5598,7 +5598,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C63">
@@ -5686,7 +5686,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C64">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C65">
@@ -5862,7 +5862,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C66">
@@ -5950,7 +5950,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C67">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C68">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C69">
@@ -6204,7 +6204,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C70">
@@ -6292,7 +6292,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C71">
@@ -6360,7 +6360,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C72">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C73">
@@ -6526,7 +6526,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C74">
@@ -6604,7 +6604,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C75">
@@ -6692,7 +6692,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C76">
@@ -6780,7 +6780,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C77">
@@ -6858,7 +6858,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C78">
@@ -6946,7 +6946,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C79">
@@ -7034,7 +7034,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C80">
@@ -7112,7 +7112,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C81">
@@ -7200,7 +7200,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C82">
@@ -7288,7 +7288,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C83">
@@ -7376,7 +7376,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C84">
@@ -7464,7 +7464,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C85">
@@ -7552,7 +7552,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C86">
@@ -7640,7 +7640,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C87">
@@ -7811,7 +7811,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C89">
@@ -7899,7 +7899,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C90">
@@ -7987,7 +7987,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C91">
@@ -8158,7 +8158,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C93">
@@ -8246,7 +8246,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C94">
@@ -8334,7 +8334,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C95">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C96">
@@ -8666,7 +8666,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C99">
@@ -8744,7 +8744,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C100">
@@ -8832,7 +8832,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C101">
@@ -8920,7 +8920,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C102">
@@ -9008,7 +9008,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C103">
@@ -9096,7 +9096,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C104">
@@ -9174,7 +9174,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C105">
@@ -9262,7 +9262,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C106">
@@ -9350,7 +9350,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C107">
@@ -9438,7 +9438,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C108">
@@ -9526,7 +9526,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C109">
@@ -9614,7 +9614,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C110">
@@ -9702,7 +9702,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C111">
@@ -9790,7 +9790,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C112">
@@ -9878,7 +9878,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C113">
@@ -10049,7 +10049,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C115">
@@ -10137,7 +10137,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C116">
@@ -10225,7 +10225,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C117">
@@ -10313,7 +10313,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C118">
@@ -10401,7 +10401,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C119">
@@ -10489,7 +10489,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C120">
@@ -10577,7 +10577,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C121">
@@ -10665,7 +10665,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C122">
@@ -10753,7 +10753,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C123">
@@ -11007,7 +11007,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C126">
@@ -11095,7 +11095,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C127">
@@ -11183,7 +11183,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C128">
@@ -11261,7 +11261,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C129">
@@ -11349,7 +11349,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C130">
@@ -11437,7 +11437,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C131">
@@ -11515,7 +11515,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C132">
@@ -11686,7 +11686,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C134">
@@ -11774,7 +11774,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C135">
@@ -11862,7 +11862,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C136">
@@ -11940,7 +11940,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C137">
@@ -12028,7 +12028,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C138">
@@ -12116,7 +12116,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C139">
@@ -12204,7 +12204,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C140">
@@ -12282,7 +12282,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C141">
@@ -12370,7 +12370,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C142">
@@ -12458,7 +12458,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C143">
@@ -12536,7 +12536,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C144">
@@ -12624,7 +12624,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C145">
@@ -12712,7 +12712,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C146">
@@ -12780,7 +12780,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C147">
@@ -12868,7 +12868,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C148">
@@ -12936,7 +12936,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C149">
@@ -13004,7 +13004,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C150">
@@ -13092,7 +13092,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C151">
@@ -13180,7 +13180,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C152">
@@ -13268,7 +13268,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C153">
@@ -13356,7 +13356,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C154">
@@ -13434,7 +13434,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C155">
@@ -13502,7 +13502,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C156">
@@ -13570,7 +13570,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C157">
@@ -13638,7 +13638,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C158">
@@ -13726,7 +13726,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C159">
@@ -13814,7 +13814,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C160">
@@ -13902,7 +13902,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C161">
@@ -13990,7 +13990,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C162">
@@ -14078,7 +14078,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C163">
@@ -14146,7 +14146,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C164">
@@ -14214,7 +14214,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C165">
@@ -14302,7 +14302,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C166">
@@ -14473,7 +14473,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C168">
@@ -14561,7 +14561,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C169">
@@ -14649,7 +14649,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C170">
@@ -14737,7 +14737,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C171">
@@ -14825,7 +14825,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C172">
@@ -14913,7 +14913,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C173">
@@ -15001,7 +15001,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C174">
@@ -15089,7 +15089,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C175">
@@ -15167,7 +15167,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C176">
@@ -15255,7 +15255,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C177">
@@ -15343,7 +15343,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C178">
@@ -15431,7 +15431,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C179">
@@ -15519,7 +15519,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C180">
@@ -15607,7 +15607,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C181">
@@ -15685,7 +15685,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C182">
@@ -15773,7 +15773,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C183">
@@ -15861,7 +15861,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C184">
@@ -15949,7 +15949,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C185">
@@ -16120,7 +16120,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C187">
@@ -16208,7 +16208,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C188">
@@ -16296,7 +16296,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C189">
@@ -16384,7 +16384,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C190">
@@ -16472,7 +16472,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C191">
@@ -16560,7 +16560,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C192">
@@ -16648,7 +16648,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C193">
@@ -16736,7 +16736,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C194">
@@ -16824,7 +16824,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C195">
@@ -16902,7 +16902,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C196">
@@ -16980,7 +16980,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C197">
@@ -17068,7 +17068,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C198">
@@ -17156,7 +17156,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C199">
@@ -17244,7 +17244,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C200">
@@ -17332,7 +17332,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C201">
@@ -17420,7 +17420,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C202">
@@ -17508,7 +17508,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C203">
@@ -17596,7 +17596,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C204">
@@ -17684,7 +17684,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C205">
@@ -17772,7 +17772,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C206">
@@ -17860,7 +17860,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C207">
@@ -17948,7 +17948,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C208">
@@ -18026,7 +18026,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C209">
@@ -18114,7 +18114,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C210">
@@ -18202,7 +18202,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C211">
@@ -18290,7 +18290,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C212">
@@ -18378,7 +18378,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C213">
@@ -18460,7 +18460,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C214">
@@ -18548,7 +18548,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C215">
@@ -18636,7 +18636,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C216">
@@ -18714,7 +18714,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C217">
@@ -18792,7 +18792,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C218">
@@ -18880,7 +18880,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C219">
@@ -18968,7 +18968,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C220">
@@ -19046,7 +19046,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C221">
@@ -19134,7 +19134,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C222">
@@ -19212,7 +19212,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C223">
@@ -19280,7 +19280,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C224">
@@ -19358,7 +19358,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C225">
@@ -19446,7 +19446,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C226">
@@ -19524,7 +19524,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C227">
@@ -19602,7 +19602,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C228">
@@ -19690,7 +19690,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C229">
@@ -19778,7 +19778,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C230">
@@ -19856,7 +19856,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C231">
@@ -19944,7 +19944,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C232">
@@ -20032,7 +20032,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="C233">
@@ -20110,7 +20110,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="C234">

</xml_diff>